<commit_message>
navegabilidad router.navigate with queryparams
</commit_message>
<xml_diff>
--- a/temp/precios-cotizaciones.xlsx
+++ b/temp/precios-cotizaciones.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20945" windowHeight="8168" activeTab="1"/>
+    <workbookView windowWidth="25134" windowHeight="10525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AUX1" sheetId="1" r:id="rId1"/>
-    <sheet name="COTIZACIONES" sheetId="2" r:id="rId2"/>
+    <sheet name="AUX3" sheetId="2" r:id="rId2"/>
     <sheet name="AUX2" sheetId="3" r:id="rId3"/>
+    <sheet name="AUX4" sheetId="4" r:id="rId4"/>
+    <sheet name="COTIZACIONES" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="72">
   <si>
     <t>ORIGEN</t>
   </si>
@@ -123,25 +125,117 @@
     <t>UNIDAD</t>
   </si>
   <si>
+    <t>MONTO FORMULAS</t>
+  </si>
+  <si>
+    <t>CANTIDAD FORMULAS</t>
+  </si>
+  <si>
+    <t>MONTO VALORES</t>
+  </si>
+  <si>
+    <t>CANTIDAD VALORES</t>
+  </si>
+  <si>
+    <t>[BTC] =  [USD]*[BTC/USD]</t>
+  </si>
+  <si>
+    <t>[USD]</t>
+  </si>
+  <si>
+    <t>[BTC]</t>
+  </si>
+  <si>
+    <t>[BTC] = [USD]/[USD/BTC]</t>
+  </si>
+  <si>
+    <t>[USD] = [ARS]*[USD/ARS]</t>
+  </si>
+  <si>
+    <t>[ARS]</t>
+  </si>
+  <si>
+    <t>[USD] = [ARS]/[ARS/USD]</t>
+  </si>
+  <si>
+    <t>[USD] = [PEN]*[USD/PEN]</t>
+  </si>
+  <si>
+    <t>[PEN]</t>
+  </si>
+  <si>
+    <t>[USD] = [PEN]/[PEN/USD]</t>
+  </si>
+  <si>
     <t>1/(BitcoinBO*CCL_MEP_COMPRA)</t>
   </si>
   <si>
+    <t>[BTC] = [ARS]*[BTC/ARS]</t>
+  </si>
+  <si>
     <t>BitcoinBO*CCL_MEP_COMPRA</t>
   </si>
   <si>
+    <t>[BTC] = [ARS]/[ARS/BTC]</t>
+  </si>
+  <si>
     <t>1/(BitcoinBO*COTIZACION_SOL_PERUANO)</t>
   </si>
   <si>
+    <t>[BTC] = [PEN]*[BTC/PEN]</t>
+  </si>
+  <si>
     <t>BitcoinBO*COTIZACION_SOL_PERUANO</t>
   </si>
   <si>
+    <t>[BTC] = [PEN]/[PEN/BTC]</t>
+  </si>
+  <si>
     <t>CCL_MEP_COMPRA/COTIZACION_SOL_PERUANO</t>
   </si>
   <si>
+    <t xml:space="preserve">[ARS] = [PEN]*[ARS/PEN]  </t>
+  </si>
+  <si>
     <t>COTIZACION_SOL_PERUANO/CCL_MEP_COMPRA</t>
   </si>
   <si>
+    <t>[ARS] = [PEN]/[PEN/ARS]</t>
+  </si>
+  <si>
     <t>COTIZACION_SOL_PERUANO*BitcoinBO</t>
+  </si>
+  <si>
+    <t>PRECIO_SS FORMULA</t>
+  </si>
+  <si>
+    <t>PRECIO_SS</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C * PRECIO_SS</t>
+  </si>
+  <si>
+    <t>M / PRECIO_SS</t>
+  </si>
+  <si>
+    <t>CASOS:
+1) Se modifica el precio sin spread =&gt; se recalcula la cantidad manteniendo constante el monto segun la formula [C]= [M]/[PRECIO_SS]</t>
+  </si>
+  <si>
+    <t>C * PRECIO_CS</t>
+  </si>
+  <si>
+    <t>M / PRECIO_CS</t>
+  </si>
+  <si>
+    <t>CASOS:
+1) [ Se modifica el precio sin spread || spread ] =&gt; se recalcula la cantidad manteniendo constante el monto segun la formula [C]= [M]/[PRECIO_SS]</t>
   </si>
 </sst>
 </file>
@@ -149,18 +243,45 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.00000000"/>
+    <numFmt numFmtId="177" formatCode="0.00000000"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -172,7 +293,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,6 +309,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -197,6 +326,21 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,21 +363,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -248,13 +377,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -263,16 +385,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,33 +402,109 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor theme="7" tint="0.599993896298105"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="7" tint="0.799981688894314"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor theme="7" tint="0.799981688894314"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="7" tint="0.599993896298105"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -323,7 +514,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,179 +628,56 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7" tint="0.399975585192419"/>
+      </left>
+      <right style="thin">
+        <color theme="7" tint="0.399975585192419"/>
+      </right>
+      <top style="thin">
+        <color theme="7" tint="0.399975585192419"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="0.399975585192419"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -520,17 +690,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -559,41 +729,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -613,157 +759,208 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="26" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="26" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1305,21 +1502,28 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88135593220339" defaultRowHeight="15.05" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.88135593220339" defaultRowHeight="15.05"/>
   <cols>
     <col min="1" max="1" width="7.32203389830508" customWidth="1"/>
     <col min="3" max="3" width="37.9067796610169" customWidth="1"/>
-    <col min="4" max="4" width="21.8728813559322" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.8728813559322" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.54237288135593" customWidth="1"/>
+    <col min="6" max="6" width="2.41525423728814" customWidth="1"/>
+    <col min="7" max="7" width="22.0932203389831" customWidth="1"/>
+    <col min="8" max="8" width="21.8474576271186" customWidth="1"/>
+    <col min="9" max="9" width="16.4322033898305" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.10169491525424" customWidth="1"/>
+    <col min="11" max="11" width="17.5338983050847" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.20338983050847" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1329,14 +1533,26 @@
       <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1346,15 +1562,34 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <f>1/D3</f>
         <v>0.000185185185185185</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="2">
+        <f>D2*K2</f>
+        <v>0.999999999999999</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="2">
+        <v>5400</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1364,14 +1599,33 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>5400</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="2">
+        <v>5400</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="2">
+        <f>I3/D3</f>
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1381,15 +1635,34 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <f>1/D6</f>
         <v>0.0111681929863748</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="2">
+        <f>K5*D5</f>
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="2">
+        <v>89.54</v>
+      </c>
+      <c r="L5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1399,14 +1672,33 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>89.54</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="2">
+        <v>89.54</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="2">
+        <f>I6/D6</f>
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1416,15 +1708,34 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <f>1/D9</f>
         <v>0.280017921146953</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="2">
+        <f>K8*D8</f>
+        <v>0.999999999999999</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="2">
+        <v>3.5712</v>
+      </c>
+      <c r="L8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1434,14 +1745,33 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>3.5712</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="2">
+        <v>3.5712</v>
+      </c>
+      <c r="J9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="2">
+        <f>I9/D9</f>
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1449,17 +1779,36 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2">
         <f>1/(D3*D6)</f>
         <v>2.0681838863657e-6</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="2">
+        <f>K11*D11</f>
+        <v>0.999999999999998</v>
+      </c>
+      <c r="J11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="2">
+        <v>483516</v>
+      </c>
+      <c r="L11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1467,17 +1816,36 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="1">
+        <v>51</v>
+      </c>
+      <c r="D12" s="2">
         <f>D3*D6</f>
         <v>483516</v>
       </c>
       <c r="E12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="2">
+        <v>483516</v>
+      </c>
+      <c r="J12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="2">
+        <f>I12/D12</f>
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1485,17 +1853,36 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="1">
+        <v>53</v>
+      </c>
+      <c r="D14" s="2">
         <f>1/(D3*D9)</f>
         <v>5.18551705827692e-5</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="G14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="2">
+        <f>K14*D14</f>
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" s="2">
+        <v>19284.48</v>
+      </c>
+      <c r="L14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1503,17 +1890,36 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1">
+        <v>55</v>
+      </c>
+      <c r="D15" s="2">
         <f>D9*D3</f>
         <v>19284.48</v>
       </c>
       <c r="E15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="2">
+        <v>19284.48</v>
+      </c>
+      <c r="J15" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="2">
+        <f>I15/D15</f>
+        <v>1</v>
+      </c>
+      <c r="L15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1521,17 +1927,36 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="1">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2">
         <f>D6/D9</f>
         <v>25.0728046594982</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="2">
+        <f>K17*D17</f>
+        <v>0.999999980118727</v>
+      </c>
+      <c r="J17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.03988385</v>
+      </c>
+      <c r="L17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1539,14 +1964,33 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="1">
+        <v>59</v>
+      </c>
+      <c r="D18" s="2">
         <f>D9/D6</f>
         <v>0.0398838507929417</v>
       </c>
       <c r="E18" t="s">
         <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.03988385</v>
+      </c>
+      <c r="J18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="2">
+        <f>I18/D18</f>
+        <v>0.999999980118728</v>
+      </c>
+      <c r="L18" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1583,7 +2027,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
@@ -1595,7 +2039,7 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <f>1/D3</f>
         <v>0.000185185185185185</v>
       </c>
@@ -1613,7 +2057,7 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>5400</v>
       </c>
       <c r="E3" t="s">
@@ -1621,7 +2065,7 @@
       </c>
     </row>
     <row r="4" spans="4:4">
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -1633,7 +2077,7 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <f>1/D6</f>
         <v>0.0111681929863748</v>
       </c>
@@ -1651,7 +2095,7 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>89.54</v>
       </c>
       <c r="E6" t="s">
@@ -1659,7 +2103,7 @@
       </c>
     </row>
     <row r="7" spans="4:4">
-      <c r="D7" s="1"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
@@ -1671,7 +2115,7 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <f>1/D9</f>
         <v>0.280017921146953</v>
       </c>
@@ -1689,7 +2133,7 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>3.5712</v>
       </c>
       <c r="E9" t="s">
@@ -1697,7 +2141,7 @@
       </c>
     </row>
     <row r="10" spans="4:4">
-      <c r="D10" s="1"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
@@ -1707,9 +2151,9 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2">
         <f>1/(D3*D6)</f>
         <v>2.0681838863657e-6</v>
       </c>
@@ -1725,9 +2169,9 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="1">
+        <v>51</v>
+      </c>
+      <c r="D12" s="2">
         <f>D3*D6</f>
         <v>483516</v>
       </c>
@@ -1736,7 +2180,7 @@
       </c>
     </row>
     <row r="13" spans="4:4">
-      <c r="D13" s="1"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
@@ -1746,9 +2190,9 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="1">
+        <v>53</v>
+      </c>
+      <c r="D14" s="2">
         <f>1/(D3*D9)</f>
         <v>5.18551705827692e-5</v>
       </c>
@@ -1764,9 +2208,9 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="1">
+        <v>61</v>
+      </c>
+      <c r="D15" s="2">
         <f>D9*D3</f>
         <v>19284.48</v>
       </c>
@@ -1775,7 +2219,7 @@
       </c>
     </row>
     <row r="16" spans="4:4">
-      <c r="D16" s="1"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
@@ -1785,9 +2229,9 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="1">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2">
         <f>D6/D9</f>
         <v>25.0728046594982</v>
       </c>
@@ -1803,9 +2247,9 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="1">
+        <v>59</v>
+      </c>
+      <c r="D18" s="2">
         <f>D9/D6</f>
         <v>0.0398838507929417</v>
       </c>
@@ -1817,4 +2261,1296 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88135593220339" defaultRowHeight="15.05"/>
+  <cols>
+    <col min="1" max="1" width="7.32203389830508" customWidth="1"/>
+    <col min="3" max="3" width="37.9067796610169" customWidth="1"/>
+    <col min="4" max="4" width="16.4322033898305" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.54237288135593" customWidth="1"/>
+    <col min="6" max="6" width="2.41525423728814" customWidth="1"/>
+    <col min="7" max="7" width="17.5254237288136" customWidth="1"/>
+    <col min="8" max="8" width="19.5338983050847" customWidth="1"/>
+    <col min="9" max="9" width="16.4322033898305" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.10169491525424" customWidth="1"/>
+    <col min="11" max="11" width="17.5338983050847" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.20338983050847" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:12">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7">
+        <f>1/D3</f>
+        <v>0.000160441277690159</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="12">
+        <f>D2*K2</f>
+        <v>0.866382899526859</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="12">
+        <v>5400</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="11">
+        <v>6232.81</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="11">
+        <v>5400</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="11">
+        <f>I3/D3</f>
+        <v>0.866382899526859</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11">
+        <f>1/D6</f>
+        <v>0.0111457868925546</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="11">
+        <f>K5*D5</f>
+        <v>0.99799375835934</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="11">
+        <v>89.54</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="12">
+        <v>89.72</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="12">
+        <v>89.54</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="12">
+        <f>I6/D6</f>
+        <v>0.99799375835934</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="12">
+        <f>1/D9</f>
+        <v>0.281357267458218</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="12">
+        <f>K8*D8</f>
+        <v>1.00478307354679</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="12">
+        <v>3.5712</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="11">
+        <v>3.5542</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="11">
+        <v>3.5712</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="11">
+        <f>I9/D9</f>
+        <v>1.00478307354679</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="14">
+        <f>1/(D3*D6)</f>
+        <v>1.78824428990369e-6</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="11">
+        <f>K11*D11</f>
+        <v>0.864644726077072</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="11">
+        <v>483516</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="12">
+        <f>D3*D6</f>
+        <v>559207.7132</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="12">
+        <v>483516</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="12">
+        <f>I12/D12</f>
+        <v>0.864644726077072</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="7">
+        <f>1/(D3*D9)</f>
+        <v>4.51413194784084e-5</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="12">
+        <f>K14*D14</f>
+        <v>0.870526872654977</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" s="12">
+        <v>19284.48</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="11">
+        <f>D9*D3</f>
+        <v>22152.653302</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="11">
+        <v>19284.48</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="11">
+        <f>I15/D15</f>
+        <v>0.870526872654977</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="11">
+        <f>D6/D9</f>
+        <v>25.2433740363514</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="11">
+        <f>K17*D17</f>
+        <v>1.00680294355973</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0.03988385</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="12">
+        <f>D9/D6</f>
+        <v>0.0396143557735176</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0.03988385</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="12">
+        <f>I18/D18</f>
+        <v>1.00680294355973</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A25:L28"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="C3:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88135593220339" defaultRowHeight="15.05"/>
+  <cols>
+    <col min="1" max="1" width="7.32203389830508" customWidth="1"/>
+    <col min="3" max="3" width="37.9067796610169" customWidth="1"/>
+    <col min="4" max="4" width="16.4322033898305" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.54237288135593" customWidth="1"/>
+    <col min="6" max="6" width="2.41525423728814" customWidth="1"/>
+    <col min="7" max="7" width="17.5254237288136" customWidth="1"/>
+    <col min="8" max="8" width="19.5338983050847" customWidth="1"/>
+    <col min="9" max="9" width="16.4322033898305" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.10169491525424" customWidth="1"/>
+    <col min="11" max="11" width="17.5338983050847" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.20338983050847" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:12">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7">
+        <f>1/D3</f>
+        <v>0.000160441277690159</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="12">
+        <f>D2*K2</f>
+        <v>0.866382899526859</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="12">
+        <v>5400</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="11">
+        <v>6232.81</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="11">
+        <v>5400</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="11">
+        <f>I3/D3</f>
+        <v>0.866382899526859</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11">
+        <f>1/D6</f>
+        <v>0.0111457868925546</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="11">
+        <f>K5*D5</f>
+        <v>0.99799375835934</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="11">
+        <v>89.54</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="12">
+        <v>89.72</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="12">
+        <v>89.54</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="12">
+        <f>I6/D6</f>
+        <v>0.99799375835934</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="12">
+        <f>1/D9</f>
+        <v>0.281357267458218</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="12">
+        <f>K8*D8</f>
+        <v>1.00478307354679</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="12">
+        <v>3.5712</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="11">
+        <v>3.5542</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="11">
+        <v>3.5712</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="11">
+        <f>I9/D9</f>
+        <v>1.00478307354679</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="14">
+        <f>1/(D3*D6)</f>
+        <v>1.78824428990369e-6</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="11">
+        <f>K11*D11</f>
+        <v>0.864644726077072</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="11">
+        <v>483516</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="12">
+        <f>D3*D6</f>
+        <v>559207.7132</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="12">
+        <v>483516</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="12">
+        <f>I12/D12</f>
+        <v>0.864644726077072</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="7">
+        <f>1/(D3*D9)</f>
+        <v>4.51413194784084e-5</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="12">
+        <f>K14*D14</f>
+        <v>0.870526872654977</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" s="12">
+        <v>19284.48</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="11">
+        <f>D9*D3</f>
+        <v>22152.653302</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="11">
+        <v>19284.48</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="11">
+        <f>I15/D15</f>
+        <v>0.870526872654977</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="11">
+        <f>D6/D9</f>
+        <v>25.2433740363514</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="11">
+        <f>K17*D17</f>
+        <v>1.00680294355973</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0.03988385</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="12">
+        <f>D9/D6</f>
+        <v>0.0396143557735176</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0.03988385</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="12">
+        <f>I18/D18</f>
+        <v>1.00680294355973</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A25:L28"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>